<commit_message>
change timezone to pakistan time
</commit_message>
<xml_diff>
--- a/employees_attendance.xlsx
+++ b/employees_attendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Employee</t>
   </si>
@@ -40,7 +40,10 @@
     <t>Nouman</t>
   </si>
   <si>
-    <t>7:50:43 PM</t>
+    <t>8:12:55 PM</t>
+  </si>
+  <si>
+    <t>8:12:56 PM</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uncomment google function call
</commit_message>
<xml_diff>
--- a/employees_attendance.xlsx
+++ b/employees_attendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Employee</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>2024-08-15</t>
+  </si>
+  <si>
+    <t>06:29:24 PM</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -520,6 +526,26 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>